<commit_message>
update omega3 (correct quantity/scale)
</commit_message>
<xml_diff>
--- a/data_fisheries_nutrients/Threshold_FAO.xlsx
+++ b/data_fisheries_nutrients/Threshold_FAO.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pos_Doc_Sinbiose\Review_within_the_group\food_security\data_fisheries_nutrients\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\MESTRADO\Nutrition\food_security-master\food_security-master\data_fisheries_nutrients\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF28ED1E-A5BA-4F4A-B2BB-97EA25693CD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Página1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -40,9 +39,6 @@
     <t>va(µg)</t>
   </si>
   <si>
-    <t>o3(mg)</t>
-  </si>
-  <si>
     <t>label</t>
   </si>
   <si>
@@ -104,12 +100,15 @@
   </si>
   <si>
     <t>mg(mg)</t>
+  </si>
+  <si>
+    <t>o3(g)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -362,33 +361,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
-        <v>18</v>
-      </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
@@ -396,10 +395,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="1">
         <v>50</v>
@@ -413,10 +412,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1">
         <v>11</v>
@@ -431,10 +430,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1">
         <v>60</v>
@@ -449,10 +448,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1">
         <v>1000</v>
@@ -467,10 +466,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" s="1">
         <v>22</v>
@@ -485,10 +484,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="1">
         <v>800</v>
@@ -499,31 +498,30 @@
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="1">
-        <v>250</v>
+        <v>2.5</v>
       </c>
       <c r="E8">
-        <f>D8/1000</f>
-        <v>0.25</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="1">
         <f>310</f>

</xml_diff>